<commit_message>
Wonders: Classical and Medieval
</commit_message>
<xml_diff>
--- a/文档/奇观.xlsx
+++ b/文档/奇观.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A523D0FD-27D4-406D-8EB9-E210AC96D33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B4D652-6B62-43D3-8ED7-34D59AD6358E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="2460" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="195">
   <si>
     <t>阿蒙森-斯科特研究站</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -648,26 +648,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>（额外）本城文化+20%。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>（额外）提前允许单位进入大洋。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>（额外）立即获得1个大音乐家。鼓舞升为2个。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>（额外）所有城市水域+2金。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>（额外）获得2个本时代随机鼓舞</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>（额外）本城+50%文化。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -708,10 +696,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>（额外）全国神祠和寺庙产出+2科研。商路加成删掉内商1鸽。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>同时获得中古全部的尤里卡。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -768,10 +752,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>（额外）每个娱乐中心提供12点旅游业绩。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>（额外）全国沼泽+2食物，</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -809,6 +789,30 @@
   </si>
   <si>
     <t>人口增长改为25%。（额外）+6食物。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（额外）每个娱乐中心提供10点旅游业绩。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（额外）全国神祠和寺庙产出+2科研。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（额外）本城20%文化。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（额外）获得2个原子时代随机鼓舞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（额外）提供20点业绩。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（额外）立即获得1个大文学家和1个大音乐家。删去鼓舞。删去本城20%文化。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -839,12 +843,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -861,7 +871,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -872,6 +882,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1151,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1202,8 +1215,8 @@
       <c r="G2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>171</v>
+      <c r="H2" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I2" s="1">
         <v>1</v>
@@ -1213,8 +1226,8 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>171</v>
+      <c r="H3" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -1224,8 +1237,8 @@
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>184</v>
+      <c r="H4" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
@@ -1253,8 +1266,8 @@
       <c r="G5" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>193</v>
+      <c r="H5" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="I5" s="1">
         <v>1</v>
@@ -1282,8 +1295,8 @@
       <c r="G6" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>192</v>
+      <c r="H6" s="4" t="s">
+        <v>187</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
@@ -1311,8 +1324,8 @@
       <c r="G7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>171</v>
+      <c r="H7" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I7" s="1">
         <v>1</v>
@@ -1331,8 +1344,8 @@
       <c r="G8" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>160</v>
+      <c r="H8" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>
@@ -1348,8 +1361,8 @@
       <c r="G9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>161</v>
+      <c r="H9" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="I9" s="1">
         <v>2</v>
@@ -1359,8 +1372,8 @@
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>182</v>
+      <c r="H10" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="I10" s="1">
         <v>2</v>
@@ -1371,10 +1384,10 @@
         <v>23</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>171</v>
+        <v>161</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I11" s="1">
         <v>2</v>
@@ -1402,8 +1415,8 @@
       <c r="G12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>156</v>
+      <c r="H12" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="I12" s="1">
         <v>2</v>
@@ -1431,8 +1444,8 @@
       <c r="G13" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>169</v>
+      <c r="H13" s="4" t="s">
+        <v>165</v>
       </c>
       <c r="I13" s="1">
         <v>2</v>
@@ -1442,8 +1455,8 @@
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>187</v>
+      <c r="H14" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="I14" s="1">
         <v>2</v>
@@ -1471,8 +1484,8 @@
       <c r="G15" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>154</v>
+      <c r="H15" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="I15" s="1">
         <v>2</v>
@@ -1488,8 +1501,8 @@
       <c r="G16" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>173</v>
+      <c r="H16" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="I16" s="1">
         <v>2</v>
@@ -1509,10 +1522,10 @@
         <v>124</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I17" s="1">
         <v>2</v>
@@ -1528,8 +1541,8 @@
       <c r="G18" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>172</v>
+      <c r="H18" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="I18" s="1">
         <v>2</v>
@@ -1551,8 +1564,8 @@
       <c r="G19" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>159</v>
+      <c r="H19" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="I19" s="1">
         <v>2</v>
@@ -1568,8 +1581,8 @@
       <c r="G20" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>170</v>
+      <c r="H20" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="I20" s="1">
         <v>2</v>
@@ -1579,8 +1592,8 @@
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>171</v>
+      <c r="H21" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I21" s="1">
         <v>3</v>
@@ -1590,8 +1603,8 @@
       <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>181</v>
+      <c r="H22" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="I22" s="1">
         <v>3</v>
@@ -1607,8 +1620,8 @@
       <c r="G23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>168</v>
+      <c r="H23" s="4" t="s">
+        <v>190</v>
       </c>
       <c r="I23" s="1">
         <v>3</v>
@@ -1624,8 +1637,8 @@
       <c r="G24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>153</v>
+      <c r="H24" s="4" t="s">
+        <v>191</v>
       </c>
       <c r="I24" s="1">
         <v>3</v>
@@ -1644,8 +1657,8 @@
       <c r="G25" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>171</v>
+      <c r="H25" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I25" s="1">
         <v>3</v>
@@ -1664,8 +1677,8 @@
       <c r="G26" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>163</v>
+      <c r="H26" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="I26" s="1">
         <v>3</v>
@@ -1687,8 +1700,8 @@
       <c r="G27" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>174</v>
+      <c r="H27" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="I27" s="1">
         <v>3</v>
@@ -1698,8 +1711,8 @@
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>186</v>
+      <c r="H28" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="I28" s="1">
         <v>3</v>
@@ -1709,8 +1722,8 @@
       <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>171</v>
+      <c r="H29" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I29" s="1">
         <v>3</v>
@@ -1720,8 +1733,8 @@
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>171</v>
+      <c r="H30" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I30" s="1">
         <v>3</v>
@@ -1732,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I31" s="1">
         <v>4</v>
@@ -1743,7 +1756,7 @@
         <v>5</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="I32" s="1">
         <v>4</v>
@@ -1763,7 +1776,7 @@
         <v>59</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I33" s="1">
         <v>4</v>
@@ -1786,7 +1799,7 @@
         <v>95</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I34" s="1">
         <v>4</v>
@@ -1797,7 +1810,7 @@
         <v>30</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I35" s="1">
         <v>4</v>
@@ -1807,8 +1820,8 @@
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>171</v>
+      <c r="H36" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I36" s="1">
         <v>4</v>
@@ -1819,7 +1832,7 @@
         <v>51</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I37" s="1">
         <v>4</v>
@@ -1830,7 +1843,7 @@
         <v>52</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="I38" s="1">
         <v>4</v>
@@ -1853,7 +1866,7 @@
         <v>56</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I39" s="1">
         <v>5</v>
@@ -1864,7 +1877,7 @@
         <v>11</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I40" s="1">
         <v>5</v>
@@ -1875,7 +1888,7 @@
         <v>12</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I41" s="1">
         <v>5</v>
@@ -1891,8 +1904,8 @@
       <c r="G42" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>171</v>
+      <c r="H42" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I42" s="1">
         <v>5</v>
@@ -1902,8 +1915,8 @@
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>171</v>
+      <c r="H43" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I43" s="1">
         <v>5</v>
@@ -1923,7 +1936,7 @@
         <v>111</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I44" s="1">
         <v>5</v>
@@ -1951,8 +1964,8 @@
       <c r="G45" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>171</v>
+      <c r="H45" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I45" s="1">
         <v>5</v>
@@ -1963,7 +1976,7 @@
         <v>46</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="I46" s="1">
         <v>5</v>
@@ -1973,8 +1986,8 @@
       <c r="A47" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>171</v>
+      <c r="H47" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="I47" s="1">
         <v>6</v>
@@ -1994,7 +2007,7 @@
         <v>77</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="I48" s="1">
         <v>6</v>
@@ -2014,7 +2027,7 @@
         <v>85</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="I49" s="1">
         <v>6</v>
@@ -2037,7 +2050,7 @@
         <v>91</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>153</v>
+        <v>193</v>
       </c>
       <c r="I50" s="1">
         <v>6</v>
@@ -2048,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I51" s="1">
         <v>7</v>
@@ -2059,7 +2072,7 @@
         <v>18</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I52" s="1">
         <v>7</v>
@@ -2070,7 +2083,7 @@
         <v>26</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="I53" s="1">
         <v>7</v>
@@ -2087,7 +2100,7 @@
         <v>146</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I54" s="1">
         <v>7</v>

</xml_diff>